<commit_message>
greedy algorithm and correct ratio
</commit_message>
<xml_diff>
--- a/CoPilot_on_Algorithm_Design/Sorting_Algorithms/Sorting Algorithms.xlsx
+++ b/CoPilot_on_Algorithm_Design/Sorting_Algorithms/Sorting Algorithms.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahvra/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GH-Dataset\Copilot_asset_liability\CopilotEvaluation\CoPilot_on_Algorithm_Design\Sorting_Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761CF7D4-110B-034A-BFF6-1D32A3046D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D39FDBA-074C-4394-853A-5CA42E6C58FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{1EB7A7BD-A671-CA46-8535-24197788BB72}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{1EB7A7BD-A671-CA46-8535-24197788BB72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sorting Algorithms" sheetId="3" r:id="rId1"/>
+    <sheet name="result" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="119">
   <si>
     <t>Algorithm</t>
   </si>
@@ -4612,12 +4613,72 @@
   <si>
     <t>O(d(n+k))</t>
   </si>
+  <si>
+    <t>inter_t1</t>
+  </si>
+  <si>
+    <t>trial_1</t>
+  </si>
+  <si>
+    <t>inter_t2</t>
+  </si>
+  <si>
+    <t>trial_2</t>
+  </si>
+  <si>
+    <t>intra</t>
+  </si>
+  <si>
+    <t>intra_st</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>algo</t>
+  </si>
+  <si>
+    <t>correct_ratio_t1</t>
+  </si>
+  <si>
+    <t>correct_ratio_t2</t>
+  </si>
+  <si>
+    <t>Bubble_Sort</t>
+  </si>
+  <si>
+    <t>Insertion_Sort</t>
+  </si>
+  <si>
+    <t>Selection_Sort</t>
+  </si>
+  <si>
+    <t>Merge_Sort</t>
+  </si>
+  <si>
+    <t>Quick_Sort</t>
+  </si>
+  <si>
+    <t>Heap_Sort</t>
+  </si>
+  <si>
+    <t>Bucket_Sort</t>
+  </si>
+  <si>
+    <t>Radix_Sort</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4635,6 +4696,14 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4667,7 +4736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4686,6 +4755,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4993,7 +5071,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5003,11 +5081,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF2443B-2976-F946-B416-88A588783960}">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
@@ -5027,7 +5105,7 @@
     <col min="21" max="21" width="77" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5092,7 +5170,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5154,7 +5232,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -5216,7 +5294,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -5278,7 +5356,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -5337,7 +5415,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -5399,7 +5477,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -5458,7 +5536,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -5517,7 +5595,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -5579,4 +5657,380 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6496FA26-B588-4C69-B003-67A057403ED9}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3">
+        <v>85.714285714285694</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>9.0909090909090899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6">
+        <v>33.3333333333333</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>16.6666666666666</v>
+      </c>
+      <c r="J7">
+        <v>16.6666666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9">
+        <v>0.66659999999999997</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>14.285714285714199</v>
+      </c>
+      <c r="J9">
+        <v>13.3333333333333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15">
+        <v>14.285714285714199</v>
+      </c>
+      <c r="C15">
+        <v>13.3333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16">
+        <v>33.3333333333333</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17">
+        <v>16.6666666666666</v>
+      </c>
+      <c r="C17">
+        <v>16.6666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>9.0909090909090899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19">
+        <v>85.714285714285694</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>